<commit_message>
Corregido fallo en scripts en la columna fecha de auditoria
</commit_message>
<xml_diff>
--- a/Excels/TLs_201812.xlsx
+++ b/Excels/TLs_201812.xlsx
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3977,7 +3977,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B79" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -4625,8 +4625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
@@ -5212,9 +5212,7 @@
       <c r="D29" s="25">
         <v>0</v>
       </c>
-      <c r="E29" s="27">
-        <v>0</v>
-      </c>
+      <c r="E29" s="27"/>
       <c r="F29" s="2">
         <v>201812</v>
       </c>
@@ -9186,9 +9184,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9324,26 +9325,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E793575B-6FDB-4D0A-9D1A-F6633906D584}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F6CEEDA-A7C8-4CA1-B28B-79033BB1D391}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c5c0a092-86e7-4d19-9228-f591611b7342"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9367,9 +9357,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F6CEEDA-A7C8-4CA1-B28B-79033BB1D391}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E793575B-6FDB-4D0A-9D1A-F6633906D584}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c5c0a092-86e7-4d19-9228-f591611b7342"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>